<commit_message>
MyISSAM load and select from product where id =
</commit_message>
<xml_diff>
--- a/mereni.xlsx
+++ b/mereni.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mira\Documents\Dokumenty\BP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mira\Documents\Dokumenty\BP\bp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>load data infile '/tmp/mirek-db/mysql/product.txt' replace into table product;</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>0.00061567</t>
+  </si>
+  <si>
+    <t>CREATE INDEX retail_price_cs_idx ON product (retailprice_cs);</t>
+  </si>
+  <si>
+    <t>load index into cache product;</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,6 +701,16 @@
         <v>49</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
product where price = 12.5
</commit_message>
<xml_diff>
--- a/mereni.xlsx
+++ b/mereni.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>load data infile '/tmp/mirek-db/mysql/product.txt' replace into table product;</t>
   </si>
@@ -180,6 +180,36 @@
   </si>
   <si>
     <t>load index into cache product;</t>
+  </si>
+  <si>
+    <t>select max(retailprice) from product;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select id from product where retailprice_cs = 12.5</t>
+  </si>
+  <si>
+    <t>0.00068527</t>
+  </si>
+  <si>
+    <t>0.00048519</t>
+  </si>
+  <si>
+    <t>0.00048550</t>
+  </si>
+  <si>
+    <t>0.00106290</t>
+  </si>
+  <si>
+    <t>0.00049251</t>
+  </si>
+  <si>
+    <t>0.00047968</t>
+  </si>
+  <si>
+    <t>0.00048119</t>
+  </si>
+  <si>
+    <t>0.00053873</t>
   </si>
 </sst>
 </file>
@@ -499,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,6 +741,40 @@
         <v>51</v>
       </c>
     </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
MyISSAM product where price
</commit_message>
<xml_diff>
--- a/mereni.xlsx
+++ b/mereni.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>load data infile '/tmp/mirek-db/mysql/product.txt' replace into table product;</t>
   </si>
@@ -210,6 +210,114 @@
   </si>
   <si>
     <t>0.00053873</t>
+  </si>
+  <si>
+    <t>select id from product where retailprice_cs = 110000</t>
+  </si>
+  <si>
+    <t>0.00968390</t>
+  </si>
+  <si>
+    <t>0.00091721</t>
+  </si>
+  <si>
+    <t>0.00074059</t>
+  </si>
+  <si>
+    <t>0.00047906</t>
+  </si>
+  <si>
+    <t>0.00070678</t>
+  </si>
+  <si>
+    <t>0.00050203</t>
+  </si>
+  <si>
+    <t>0.00067805</t>
+  </si>
+  <si>
+    <t>0.00053893</t>
+  </si>
+  <si>
+    <t>select id from product where retailprice_cs = 2932650</t>
+  </si>
+  <si>
+    <t>0.00050963</t>
+  </si>
+  <si>
+    <t>0.00051144</t>
+  </si>
+  <si>
+    <t>0.00767151</t>
+  </si>
+  <si>
+    <t>0.00047020</t>
+  </si>
+  <si>
+    <t>0.00053813</t>
+  </si>
+  <si>
+    <t>0.00068424</t>
+  </si>
+  <si>
+    <t>0.00049065</t>
+  </si>
+  <si>
+    <t>0.00051151</t>
+  </si>
+  <si>
+    <t>select id from product where retailprice_cs = 1855875</t>
+  </si>
+  <si>
+    <t>0.00050368</t>
+  </si>
+  <si>
+    <t>0.00046416</t>
+  </si>
+  <si>
+    <t>0.00046276</t>
+  </si>
+  <si>
+    <t>0.00049457</t>
+  </si>
+  <si>
+    <t>0.00046781</t>
+  </si>
+  <si>
+    <t>0.00049790</t>
+  </si>
+  <si>
+    <t>0.00059695</t>
+  </si>
+  <si>
+    <t>0.00063842</t>
+  </si>
+  <si>
+    <t>select id from product where retailprice_cs = 954375</t>
+  </si>
+  <si>
+    <t>0.00062934</t>
+  </si>
+  <si>
+    <t>0.00064824</t>
+  </si>
+  <si>
+    <t>0.00058874</t>
+  </si>
+  <si>
+    <t>0.00057954</t>
+  </si>
+  <si>
+    <t>0.00066041</t>
+  </si>
+  <si>
+    <t>0.00068109</t>
+  </si>
+  <si>
+    <t>0.00054907</t>
+  </si>
+  <si>
+    <t>0.00071128</t>
   </si>
 </sst>
 </file>
@@ -529,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +883,122 @@
         <v>61</v>
       </c>
     </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" t="s">
+        <v>78</v>
+      </c>
+      <c r="I20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" t="s">
+        <v>86</v>
+      </c>
+      <c r="H21" t="s">
+        <v>87</v>
+      </c>
+      <c r="I21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22" t="s">
+        <v>96</v>
+      </c>
+      <c r="I22" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
MyIssam product were  internal_number
</commit_message>
<xml_diff>
--- a/mereni.xlsx
+++ b/mereni.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
   <si>
     <t>load data infile '/tmp/mirek-db/mysql/product.txt' replace into table product;</t>
   </si>
@@ -318,6 +318,141 @@
   </si>
   <si>
     <t>0.00071128</t>
+  </si>
+  <si>
+    <t>select id from product where internal_number = "0 001 108 211"</t>
+  </si>
+  <si>
+    <t>0.00068110</t>
+  </si>
+  <si>
+    <t>0.00076386</t>
+  </si>
+  <si>
+    <t>0.00187179</t>
+  </si>
+  <si>
+    <t>0.00066529</t>
+  </si>
+  <si>
+    <t>0.00075340</t>
+  </si>
+  <si>
+    <t>0.00087936</t>
+  </si>
+  <si>
+    <t>0.00067745</t>
+  </si>
+  <si>
+    <t>0.00072914</t>
+  </si>
+  <si>
+    <t>select id from product where internal_number = "QB WS 0344 A"</t>
+  </si>
+  <si>
+    <t>0.00054724</t>
+  </si>
+  <si>
+    <t>0.00049655</t>
+  </si>
+  <si>
+    <t>0.00050429</t>
+  </si>
+  <si>
+    <t>0.00050158</t>
+  </si>
+  <si>
+    <t>0.00049735</t>
+  </si>
+  <si>
+    <t>0.00051131</t>
+  </si>
+  <si>
+    <t>0.00046639</t>
+  </si>
+  <si>
+    <t>0.00052117</t>
+  </si>
+  <si>
+    <t>select id from product where internal_number = "SD 0 986 474 332"</t>
+  </si>
+  <si>
+    <t>0.00077904</t>
+  </si>
+  <si>
+    <t>0.00065300</t>
+  </si>
+  <si>
+    <t>0.00049882</t>
+  </si>
+  <si>
+    <t>0.00063806</t>
+  </si>
+  <si>
+    <t>0.00050456</t>
+  </si>
+  <si>
+    <t>0.00045716</t>
+  </si>
+  <si>
+    <t>0.00051399</t>
+  </si>
+  <si>
+    <t>0.00090095</t>
+  </si>
+  <si>
+    <t>select id from product where internal_number = "0 132 801 002"</t>
+  </si>
+  <si>
+    <t>0.00101897</t>
+  </si>
+  <si>
+    <t>0.00067223</t>
+  </si>
+  <si>
+    <t>0.00050217</t>
+  </si>
+  <si>
+    <t>0.00053300</t>
+  </si>
+  <si>
+    <t>0.00059784</t>
+  </si>
+  <si>
+    <t>0.00050421</t>
+  </si>
+  <si>
+    <t>0.00249899</t>
+  </si>
+  <si>
+    <t>0.00057782</t>
+  </si>
+  <si>
+    <t>select id from product where internal_number = "9XX 340 369-011"</t>
+  </si>
+  <si>
+    <t>0.00058355</t>
+  </si>
+  <si>
+    <t>0.00312450</t>
+  </si>
+  <si>
+    <t>0.00057385</t>
+  </si>
+  <si>
+    <t>0.00053378</t>
+  </si>
+  <si>
+    <t>0.00051494</t>
+  </si>
+  <si>
+    <t>0.00056448</t>
+  </si>
+  <si>
+    <t>0.00056384</t>
+  </si>
+  <si>
+    <t>0.00053007</t>
   </si>
 </sst>
 </file>
@@ -637,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,6 +1134,151 @@
         <v>97</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" t="s">
+        <v>111</v>
+      </c>
+      <c r="F25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" t="s">
+        <v>113</v>
+      </c>
+      <c r="H25" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" t="s">
+        <v>121</v>
+      </c>
+      <c r="G26" t="s">
+        <v>122</v>
+      </c>
+      <c r="H26" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" t="s">
+        <v>131</v>
+      </c>
+      <c r="H27" t="s">
+        <v>132</v>
+      </c>
+      <c r="I27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G28" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
text o výběru enginů
</commit_message>
<xml_diff>
--- a/mereni.xlsx
+++ b/mereni.xlsx
@@ -560,7 +560,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="9885" topLeftCell="S1" activePane="topRight"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="Y2" sqref="Y2"/>
+      <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,6 +727,15 @@
       <c r="X2" s="2">
         <v>3.4216435185185183E-3</v>
       </c>
+      <c r="Y2" s="2">
+        <v>3.3328703703703702E-3</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>3.650462962962963E-3</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>3.3495370370370367E-3</v>
+      </c>
       <c r="AC2" t="s">
         <v>15</v>
       </c>

</xml_diff>